<commit_message>
Nom, ID, Canonical 37604f1e96c95306324e18f0a5457b5f108ad7ba
</commit_message>
<xml_diff>
--- a/1-définir-le-nom-id-et-canonical-de-lig/ig/CodeSystem-competence-code-system.xlsx
+++ b/1-définir-le-nom-id-et-canonical-de-lig/ig/CodeSystem-competence-code-system.xlsx
@@ -24,7 +24,7 @@
     <t>URL</t>
   </si>
   <si>
-    <t>https://interop.esante.gouv.fr/ig/fhir/[code]/CodeSystem/competence-code-system</t>
+    <t>https://interop.esante.gouv.fr/ig/fhir/nde/CodeSystem/competence-code-system</t>
   </si>
   <si>
     <t>Version</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2026-01-06T10:03:56+00:00</t>
+    <t>2026-01-06T10:14:23+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>